<commit_message>
Adicionado envio do relatório por e-mail
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Palavra Chave</t>
   </si>
@@ -20,9 +20,6 @@
   </si>
   <si>
     <t>Posição</t>
-  </si>
-  <si>
-    <t>Teste</t>
   </si>
 </sst>
 </file>
@@ -399,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -413,83 +410,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Realizando envio do relatório da busca das palavras chave por e-mail
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -11,7 +11,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Usiwal</t>
+  </si>
+  <si>
+    <t>usiwal.com.br</t>
+  </si>
   <si>
     <t>Palavra Chave</t>
   </si>
@@ -20,19 +26,32 @@
   </si>
   <si>
     <t>Posição</t>
+  </si>
+  <si>
+    <t>Cilindros Hidráulicos De Alta Pressão</t>
+  </si>
+  <si>
+    <t>Cilindros Hidráulicos 700 Bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="18243B"/>
+      <family val="4"/>
+      <sz val="24"/>
+      <name val="Arial Black"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,8 +74,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,21 +421,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="100" customWidth="1"/>
+    <col min="2" max="3" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionado envio de zip das imagens por e-mail
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Usiwal</t>
-  </si>
-  <si>
-    <t>usiwal.com.br</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>Gráfica Vektra</t>
+  </si>
+  <si>
+    <t>graficavektra.com.br</t>
   </si>
   <si>
     <t>Palavra Chave</t>
@@ -28,10 +28,19 @@
     <t>Posição</t>
   </si>
   <si>
-    <t>Cilindros Hidráulicos De Alta Pressão</t>
-  </si>
-  <si>
-    <t>Cilindros Hidráulicos 700 Bar</t>
+    <t>Gráfica para convites especiais</t>
+  </si>
+  <si>
+    <t>Gráfica ecológica</t>
+  </si>
+  <si>
+    <t>Gráfica digital</t>
+  </si>
+  <si>
+    <t>Não encontrado</t>
+  </si>
+  <si>
+    <t>Gráfica digital em sp</t>
   </si>
 </sst>
 </file>
@@ -421,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="100" customWidth="1"/>
@@ -461,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,7 +481,29 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionada pesquisa pela url
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>Gráfica Vektra</t>
-  </si>
-  <si>
-    <t>graficavektra.com.br</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>SmartFire</t>
+  </si>
+  <si>
+    <t>smartfire.com.br</t>
   </si>
   <si>
     <t>Palavra Chave</t>
@@ -28,19 +28,7 @@
     <t>Posição</t>
   </si>
   <si>
-    <t>Gráfica para convites especiais</t>
-  </si>
-  <si>
-    <t>Gráfica ecológica</t>
-  </si>
-  <si>
-    <t>Gráfica digital</t>
-  </si>
-  <si>
-    <t>Não encontrado</t>
-  </si>
-  <si>
-    <t>Gráfica digital em sp</t>
+    <t>Global Fire Manutenção</t>
   </si>
 </sst>
 </file>
@@ -430,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="100" customWidth="1"/>
@@ -470,40 +458,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
         <v>1</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -511,6 +466,9 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Nova versão da aplicação
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -28,10 +28,10 @@
     <t>Posição</t>
   </si>
   <si>
-    <t>Cilindros Hidráulicos</t>
-  </si>
-  <si>
     <t>Cilindros Hidráulicos De Alta Pressão</t>
+  </si>
+  <si>
+    <t>Cilindros Hidráulicos 700 Bar</t>
   </si>
 </sst>
 </file>
@@ -458,10 +458,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correção no posicionamento de palavras não localizadas.
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -13,10 +13,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Usiwal</t>
-  </si>
-  <si>
-    <t>usiwal.com.br</t>
+    <t>SmartFire</t>
+  </si>
+  <si>
+    <t>smartfire.com.br</t>
   </si>
   <si>
     <t>Palavra Chave</t>
@@ -28,10 +28,10 @@
     <t>Posição</t>
   </si>
   <si>
-    <t>Cilindros Hidráulicos De Alta Pressão</t>
-  </si>
-  <si>
-    <t>Cilindros Hidráulicos 700 Bar</t>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Não encontrado</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="100" customWidth="1"/>
@@ -458,21 +458,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +471,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Alterado e-mail para envio
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>SmartFire</t>
-  </si>
-  <si>
-    <t>smartfire.com.br</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Acustica Atos</t>
+  </si>
+  <si>
+    <t>acusticatos.com.br</t>
   </si>
   <si>
     <t>Palavra Chave</t>
@@ -28,10 +28,7 @@
     <t>Posição</t>
   </si>
   <si>
-    <t>Teste</t>
-  </si>
-  <si>
-    <t>Não encontrado</t>
+    <t>Tratamento acústico com espuma acústica sonex</t>
   </si>
 </sst>
 </file>
@@ -458,10 +455,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>